<commit_message>
HCT595, audio shield sockets
</commit_message>
<xml_diff>
--- a/pins.xlsx
+++ b/pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repos\mcguitarpedal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155D452B-C145-492A-A07D-DED548068B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3303AA2E-B222-435F-A8A3-A6CDEA9C24BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7E72EA4-AA0D-4192-98B3-6275BC401633}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="143">
   <si>
     <t>Audio Shield</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>LED_STR</t>
+  </si>
+  <si>
+    <t>LED_PWM</t>
+  </si>
+  <si>
+    <t>BACKLIGHT_PWM</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -717,16 +726,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -763,7 +772,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>236718</xdr:colOff>
+      <xdr:colOff>244338</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>37461</xdr:rowOff>
     </xdr:to>
@@ -806,9 +815,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>70708</xdr:colOff>
+      <xdr:colOff>59278</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>184851</xdr:rowOff>
+      <xdr:rowOff>173421</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1165,8 +1174,8 @@
   </sheetPr>
   <dimension ref="G10:AA152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L127" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O149" sqref="O149"/>
+    <sheetView tabSelected="1" topLeftCell="L123" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M137" sqref="M137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,10 +1205,10 @@
         <v>2</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="26" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1211,90 +1220,90 @@
         <v>3</v>
       </c>
       <c r="I11" s="6"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="25" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="8">
         <v>23</v>
       </c>
       <c r="I12" s="8"/>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G13" s="27"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
     </row>
     <row r="14" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="25" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="8">
         <v>21</v>
       </c>
       <c r="I14" s="8"/>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="K14" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G15" s="27"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="9"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
     </row>
     <row r="16" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="25" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="8">
         <v>20</v>
       </c>
       <c r="I16" s="8"/>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G17" s="27"/>
+      <c r="G17" s="25"/>
       <c r="H17" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="25" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="8">
         <v>7</v>
       </c>
       <c r="I18" s="8"/>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="25" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="7" t="s">
@@ -1302,25 +1311,25 @@
       </c>
     </row>
     <row r="19" spans="7:11" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G19" s="27"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="25"/>
       <c r="K19" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="25" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="8">
         <v>8</v>
       </c>
       <c r="I20" s="8"/>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="25" t="s">
         <v>23</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -1328,12 +1337,12 @@
       </c>
     </row>
     <row r="21" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G21" s="27"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="27"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="10" t="s">
         <v>25</v>
       </c>
@@ -1369,124 +1378,124 @@
       </c>
     </row>
     <row r="24" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="28">
         <v>13</v>
       </c>
-      <c r="I24" s="26"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="25" t="s">
+      <c r="K24" s="27" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
       <c r="J25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="25"/>
+      <c r="K25" s="27"/>
     </row>
     <row r="26" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="28">
         <v>12</v>
       </c>
-      <c r="I26" s="26"/>
+      <c r="I26" s="28"/>
       <c r="J26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="25" t="s">
+      <c r="K26" s="27" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
       <c r="J27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="25"/>
+      <c r="K27" s="27"/>
     </row>
     <row r="28" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="28">
         <v>11</v>
       </c>
-      <c r="I28" s="26"/>
+      <c r="I28" s="28"/>
       <c r="J28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="25" t="s">
+      <c r="K28" s="27" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
       <c r="J29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K29" s="25"/>
+      <c r="K29" s="27"/>
     </row>
     <row r="30" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G30" s="25" t="s">
+      <c r="G30" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="28">
         <v>10</v>
       </c>
-      <c r="I30" s="26"/>
+      <c r="I30" s="28"/>
       <c r="J30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="25" t="s">
+      <c r="K30" s="27" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G31" s="25"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
       <c r="J31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K31" s="25"/>
+      <c r="K31" s="27"/>
     </row>
     <row r="32" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="26">
+      <c r="H32" s="28">
         <v>6</v>
       </c>
-      <c r="I32" s="26"/>
+      <c r="I32" s="28"/>
       <c r="J32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="25" t="s">
+      <c r="K32" s="27" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" spans="7:27" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G33" s="25"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
       <c r="J33" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K33" s="25"/>
+      <c r="K33" s="27"/>
     </row>
     <row r="34" spans="7:27" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="G34" s="7" t="s">
@@ -3300,8 +3309,8 @@
       </c>
     </row>
     <row r="134" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="O134" t="s">
-        <v>137</v>
+      <c r="O134" s="24" t="s">
+        <v>132</v>
       </c>
       <c r="P134" t="s">
         <v>91</v>
@@ -3366,6 +3375,9 @@
       </c>
     </row>
     <row r="137" spans="13:22" x14ac:dyDescent="0.3">
+      <c r="M137" t="s">
+        <v>142</v>
+      </c>
       <c r="O137" t="s">
         <v>135</v>
       </c>
@@ -3384,7 +3396,7 @@
         <v>87</v>
       </c>
       <c r="V137" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="138" spans="13:22" x14ac:dyDescent="0.3">
@@ -3420,7 +3432,7 @@
     </row>
     <row r="140" spans="13:22" x14ac:dyDescent="0.3">
       <c r="O140" s="24" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="P140" t="s">
         <v>77</v>
@@ -3475,7 +3487,7 @@
         <v>9</v>
       </c>
       <c r="V142" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="143" spans="13:22" x14ac:dyDescent="0.3">
@@ -3607,8 +3619,8 @@
       <c r="T149">
         <v>2</v>
       </c>
-      <c r="V149" t="s">
-        <v>127</v>
+      <c r="V149" s="24" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="150" spans="15:22" x14ac:dyDescent="0.3">
@@ -3653,6 +3665,26 @@
     <sortCondition ref="L75:L98"/>
   </sortState>
   <mergeCells count="35">
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="K26:K27"/>
     <mergeCell ref="G20:G21"/>
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="J10:J11"/>
@@ -3668,26 +3700,6 @@
     <mergeCell ref="K16:K17"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="J18:J19"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="K30:K31"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Backlight control, PWR leds
</commit_message>
<xml_diff>
--- a/pins.xlsx
+++ b/pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repos\mcguitarpedal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266560E5-CBD9-41A1-BC61-E9256C4BD8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0737CCAF-1520-4847-A74E-4E1E18D0A72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7E72EA4-AA0D-4192-98B3-6275BC401633}"/>
   </bookViews>
@@ -726,16 +726,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1174,8 +1174,8 @@
   </sheetPr>
   <dimension ref="G10:AA152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L123" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M137" sqref="M137"/>
+    <sheetView tabSelected="1" topLeftCell="K123" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N136" sqref="N136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,10 +1205,10 @@
         <v>2</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1220,90 +1220,90 @@
         <v>3</v>
       </c>
       <c r="I11" s="6"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="27" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="8">
         <v>23</v>
       </c>
       <c r="I12" s="8"/>
-      <c r="J12" s="25" t="s">
+      <c r="J12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="25" t="s">
+      <c r="K12" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G13" s="25"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
     </row>
     <row r="14" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="27" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="8">
         <v>21</v>
       </c>
       <c r="I14" s="8"/>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="K14" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G15" s="25"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="9"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="27" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="8">
         <v>20</v>
       </c>
       <c r="I16" s="8"/>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="25" t="s">
+      <c r="K16" s="27" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G17" s="25"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="27" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="8">
         <v>7</v>
       </c>
       <c r="I18" s="8"/>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="27" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="7" t="s">
@@ -1311,25 +1311,25 @@
       </c>
     </row>
     <row r="19" spans="7:11" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G19" s="25"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="25"/>
+      <c r="J19" s="27"/>
       <c r="K19" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="27" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="8">
         <v>8</v>
       </c>
       <c r="I20" s="8"/>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="27" t="s">
         <v>23</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -1337,12 +1337,12 @@
       </c>
     </row>
     <row r="21" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G21" s="25"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="25"/>
+      <c r="J21" s="27"/>
       <c r="K21" s="10" t="s">
         <v>25</v>
       </c>
@@ -1378,124 +1378,124 @@
       </c>
     </row>
     <row r="24" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="26">
         <v>13</v>
       </c>
-      <c r="I24" s="28"/>
+      <c r="I24" s="26"/>
       <c r="J24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="27" t="s">
+      <c r="K24" s="25" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G25" s="27"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
       <c r="J25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="27"/>
+      <c r="K25" s="25"/>
     </row>
     <row r="26" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="28">
+      <c r="H26" s="26">
         <v>12</v>
       </c>
-      <c r="I26" s="28"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="27" t="s">
+      <c r="K26" s="25" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
       <c r="J27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="27"/>
+      <c r="K27" s="25"/>
     </row>
     <row r="28" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G28" s="27" t="s">
+      <c r="G28" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="28">
+      <c r="H28" s="26">
         <v>11</v>
       </c>
-      <c r="I28" s="28"/>
+      <c r="I28" s="26"/>
       <c r="J28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="27" t="s">
+      <c r="K28" s="25" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
       <c r="J29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K29" s="27"/>
+      <c r="K29" s="25"/>
     </row>
     <row r="30" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="28">
+      <c r="H30" s="26">
         <v>10</v>
       </c>
-      <c r="I30" s="28"/>
+      <c r="I30" s="26"/>
       <c r="J30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="27" t="s">
+      <c r="K30" s="25" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
       <c r="J31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K31" s="27"/>
+      <c r="K31" s="25"/>
     </row>
     <row r="32" spans="7:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G32" s="27" t="s">
+      <c r="G32" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="28">
+      <c r="H32" s="26">
         <v>6</v>
       </c>
-      <c r="I32" s="28"/>
+      <c r="I32" s="26"/>
       <c r="J32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="27" t="s">
+      <c r="K32" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" spans="7:27" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
       <c r="J33" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K33" s="27"/>
+      <c r="K33" s="25"/>
     </row>
     <row r="34" spans="7:27" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="G34" s="7" t="s">
@@ -3309,8 +3309,8 @@
       </c>
     </row>
     <row r="134" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="O134" s="24" t="s">
-        <v>132</v>
+      <c r="O134" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="P134" t="s">
         <v>91</v>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="140" spans="13:22" x14ac:dyDescent="0.3">
       <c r="O140" s="24" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="P140" t="s">
         <v>77</v>
@@ -3453,8 +3453,8 @@
       <c r="M141" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="O141" s="2" t="s">
-        <v>111</v>
+      <c r="O141" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="P141" t="s">
         <v>78</v>
@@ -3472,8 +3472,8 @@
       </c>
     </row>
     <row r="142" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="O142" s="19" t="s">
-        <v>123</v>
+      <c r="O142" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="P142" s="19" t="s">
         <v>86</v>
@@ -3665,26 +3665,6 @@
     <sortCondition ref="L75:L98"/>
   </sortState>
   <mergeCells count="35">
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="K26:K27"/>
     <mergeCell ref="G20:G21"/>
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="J10:J11"/>
@@ -3700,6 +3680,26 @@
     <mergeCell ref="K16:K17"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="J18:J19"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="K30:K31"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Front plate design 4
</commit_message>
<xml_diff>
--- a/pins.xlsx
+++ b/pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repos\mcguitarpedal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE3884A-ACFF-47BE-AF8A-CD8A51896956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D72B401-E6ED-43CE-A5D1-367B5D548E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E7E72EA4-AA0D-4192-98B3-6275BC401633}"/>
   </bookViews>
@@ -758,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -800,18 +800,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -864,26 +852,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -894,10 +878,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1056,14 +1048,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>5257</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>170578</xdr:rowOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>7291</xdr:colOff>
       <xdr:row>178</xdr:row>
-      <xdr:rowOff>161700</xdr:rowOff>
+      <xdr:rowOff>161699</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1080,13 +1072,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="4424" t="37904" r="6822" b="39630"/>
+        <a:srcRect l="4423" t="37904" r="8460" b="39630"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="14952539" y="31493261"/>
-          <a:ext cx="4814913" cy="1260991"/>
+          <a:off x="14084336" y="30897970"/>
+          <a:ext cx="4609875" cy="1259334"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1420,7 +1412,7 @@
   </sheetPr>
   <dimension ref="G10:AC178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L150" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F146" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N154" sqref="N154:X179"/>
     </sheetView>
   </sheetViews>
@@ -1435,11 +1427,11 @@
     <col min="14" max="14" width="4" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="4.109375" customWidth="1"/>
-    <col min="17" max="17" width="11.109375" style="36" customWidth="1"/>
+    <col min="17" max="17" width="11.109375" style="32" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.44140625" customWidth="1"/>
-    <col min="22" max="22" width="4.88671875" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.88671875" style="25" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.77734375" customWidth="1"/>
     <col min="25" max="25" width="14.109375" bestFit="1" customWidth="1"/>
@@ -1453,14 +1445,14 @@
         <v>2</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
     </row>
     <row r="11" spans="7:13" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="5" t="s">
@@ -1470,154 +1462,154 @@
         <v>3</v>
       </c>
       <c r="I11" s="6"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="53" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="8">
         <v>23</v>
       </c>
       <c r="I12" s="8"/>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
     </row>
     <row r="13" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G13" s="27"/>
+      <c r="G13" s="53"/>
       <c r="H13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
     </row>
     <row r="14" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="53" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="8">
         <v>21</v>
       </c>
       <c r="I14" s="8"/>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="K14" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
     </row>
     <row r="15" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G15" s="27"/>
+      <c r="G15" s="53"/>
       <c r="H15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="9"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
     </row>
     <row r="16" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="53" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="8">
         <v>20</v>
       </c>
       <c r="I16" s="8"/>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
     </row>
     <row r="17" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G17" s="27"/>
+      <c r="G17" s="53"/>
       <c r="H17" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
     </row>
     <row r="18" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="53" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="8">
         <v>7</v>
       </c>
       <c r="I18" s="8"/>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="53" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
     </row>
     <row r="19" spans="7:13" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G19" s="27"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="53"/>
       <c r="K19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
     </row>
     <row r="20" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="53" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="8">
         <v>8</v>
       </c>
       <c r="I20" s="8"/>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
     </row>
     <row r="21" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G21" s="27"/>
+      <c r="G21" s="53"/>
       <c r="H21" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="27"/>
+      <c r="J21" s="53"/>
       <c r="K21" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
     </row>
     <row r="22" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G22" s="7" t="s">
@@ -1633,8 +1625,8 @@
       <c r="K22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
     </row>
     <row r="23" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G23" s="7" t="s">
@@ -1650,148 +1642,148 @@
       <c r="K23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
     </row>
     <row r="24" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="56">
         <v>13</v>
       </c>
-      <c r="I24" s="26"/>
+      <c r="I24" s="56"/>
       <c r="J24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="25" t="s">
+      <c r="K24" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
     </row>
     <row r="25" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
       <c r="J25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
     </row>
     <row r="26" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="56">
         <v>12</v>
       </c>
-      <c r="I26" s="26"/>
+      <c r="I26" s="56"/>
       <c r="J26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="25" t="s">
+      <c r="K26" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
     </row>
     <row r="27" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
       <c r="J27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="25"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
     </row>
     <row r="28" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="56">
         <v>11</v>
       </c>
-      <c r="I28" s="26"/>
+      <c r="I28" s="56"/>
       <c r="J28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="25" t="s">
+      <c r="K28" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
     </row>
     <row r="29" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
       <c r="J29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="50"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
     </row>
     <row r="30" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G30" s="25" t="s">
+      <c r="G30" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="56">
         <v>10</v>
       </c>
-      <c r="I30" s="26"/>
+      <c r="I30" s="56"/>
       <c r="J30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="25" t="s">
+      <c r="K30" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
     </row>
     <row r="31" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G31" s="25"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K31" s="25"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
     </row>
     <row r="32" spans="7:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="26">
+      <c r="H32" s="56">
         <v>6</v>
       </c>
-      <c r="I32" s="26"/>
+      <c r="I32" s="56"/>
       <c r="J32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="25" t="s">
+      <c r="K32" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
     </row>
     <row r="33" spans="7:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="G33" s="25"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
       <c r="J33" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K33" s="25"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
     </row>
     <row r="34" spans="7:29" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="G34" s="7" t="s">
@@ -1807,8 +1799,8 @@
       <c r="K34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
     </row>
     <row r="40" spans="7:29" x14ac:dyDescent="0.3">
       <c r="G40" s="12" t="s">
@@ -1823,12 +1815,12 @@
       <c r="N40">
         <v>62</v>
       </c>
-      <c r="S40" s="30" t="s">
+      <c r="S40" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
-      <c r="V40" s="30" t="s">
+      <c r="V40" s="26" t="s">
         <v>52</v>
       </c>
       <c r="AB40">
@@ -1848,12 +1840,12 @@
       <c r="N41">
         <v>61</v>
       </c>
-      <c r="S41" s="31">
+      <c r="S41" s="27">
         <v>0</v>
       </c>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
-      <c r="V41" s="34"/>
+      <c r="V41" s="30"/>
       <c r="W41" s="3" t="s">
         <v>49</v>
       </c>
@@ -1871,12 +1863,12 @@
       <c r="N42">
         <v>60</v>
       </c>
-      <c r="S42" s="31">
+      <c r="S42" s="27">
         <v>1</v>
       </c>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
-      <c r="V42" s="30" t="s">
+      <c r="V42" s="26" t="s">
         <v>50</v>
       </c>
       <c r="AB42">
@@ -1896,12 +1888,12 @@
       <c r="N43">
         <v>59</v>
       </c>
-      <c r="S43" s="31">
+      <c r="S43" s="27">
         <v>2</v>
       </c>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
-      <c r="V43" s="29">
+      <c r="V43" s="25">
         <v>23</v>
       </c>
       <c r="W43" t="s">
@@ -1924,12 +1916,12 @@
       <c r="N44">
         <v>58</v>
       </c>
-      <c r="S44" s="31">
+      <c r="S44" s="27">
         <v>3</v>
       </c>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
-      <c r="V44" s="29">
+      <c r="V44" s="25">
         <v>22</v>
       </c>
       <c r="W44" s="19" t="s">
@@ -1952,12 +1944,12 @@
       <c r="N45">
         <v>57</v>
       </c>
-      <c r="S45" s="31">
+      <c r="S45" s="27">
         <v>4</v>
       </c>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
-      <c r="V45" s="29">
+      <c r="V45" s="25">
         <v>21</v>
       </c>
       <c r="W45" t="s">
@@ -1980,12 +1972,12 @@
       <c r="N46">
         <v>56</v>
       </c>
-      <c r="S46" s="31">
+      <c r="S46" s="27">
         <v>5</v>
       </c>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
-      <c r="V46" s="29">
+      <c r="V46" s="25">
         <v>20</v>
       </c>
       <c r="W46" t="s">
@@ -2008,15 +2000,15 @@
       <c r="N47">
         <v>55</v>
       </c>
-      <c r="Q47" s="37" t="s">
+      <c r="Q47" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="S47" s="32">
+      <c r="S47" s="28">
         <v>6</v>
       </c>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
-      <c r="V47" s="29">
+      <c r="V47" s="25">
         <v>19</v>
       </c>
       <c r="W47" t="s">
@@ -2042,15 +2034,15 @@
       <c r="N48">
         <v>54</v>
       </c>
-      <c r="Q48" s="38" t="s">
+      <c r="Q48" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="S48" s="32">
+      <c r="S48" s="28">
         <v>7</v>
       </c>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
-      <c r="V48" s="29">
+      <c r="V48" s="25">
         <v>18</v>
       </c>
       <c r="W48" t="s">
@@ -2073,15 +2065,15 @@
       <c r="N49">
         <v>53</v>
       </c>
-      <c r="Q49" s="38" t="s">
+      <c r="Q49" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="S49" s="32">
+      <c r="S49" s="28">
         <v>8</v>
       </c>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
-      <c r="V49" s="29">
+      <c r="V49" s="25">
         <v>17</v>
       </c>
       <c r="W49" s="19" t="s">
@@ -2104,12 +2096,12 @@
       <c r="P50" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="S50" s="33">
+      <c r="S50" s="29">
         <v>9</v>
       </c>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
-      <c r="V50" s="29">
+      <c r="V50" s="25">
         <v>16</v>
       </c>
       <c r="W50" s="19" t="s">
@@ -2132,15 +2124,15 @@
       <c r="N51">
         <v>51</v>
       </c>
-      <c r="Q51" s="38" t="s">
+      <c r="Q51" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="S51" s="29">
+      <c r="S51" s="25">
         <v>10</v>
       </c>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
-      <c r="V51" s="29">
+      <c r="V51" s="25">
         <v>15</v>
       </c>
       <c r="W51" s="19" t="s">
@@ -2163,15 +2155,15 @@
       <c r="N52">
         <v>50</v>
       </c>
-      <c r="Q52" s="38" t="s">
+      <c r="Q52" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="S52" s="33">
+      <c r="S52" s="29">
         <v>11</v>
       </c>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
-      <c r="V52" s="29">
+      <c r="V52" s="25">
         <v>14</v>
       </c>
       <c r="W52" s="19" t="s">
@@ -2191,15 +2183,15 @@
       <c r="N53">
         <v>49</v>
       </c>
-      <c r="Q53" s="38" t="s">
+      <c r="Q53" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="S53" s="33">
+      <c r="S53" s="29">
         <v>12</v>
       </c>
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
-      <c r="V53" s="33">
+      <c r="V53" s="29">
         <v>13</v>
       </c>
       <c r="W53" t="s">
@@ -2225,12 +2217,12 @@
       <c r="N54">
         <v>48</v>
       </c>
-      <c r="S54" s="30" t="s">
+      <c r="S54" s="26" t="s">
         <v>50</v>
       </c>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
-      <c r="V54" s="30" t="s">
+      <c r="V54" s="26" t="s">
         <v>49</v>
       </c>
       <c r="AB54">
@@ -2241,18 +2233,18 @@
       <c r="N55">
         <v>47</v>
       </c>
-      <c r="Q55" s="37" t="s">
+      <c r="Q55" s="33" t="s">
         <v>111</v>
       </c>
       <c r="R55" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="29">
+      <c r="S55" s="25">
         <v>24</v>
       </c>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
-      <c r="V55" s="33">
+      <c r="V55" s="29">
         <v>41</v>
       </c>
       <c r="W55" t="s">
@@ -2278,12 +2270,12 @@
       <c r="R56" t="s">
         <v>88</v>
       </c>
-      <c r="S56" s="29">
+      <c r="S56" s="25">
         <v>25</v>
       </c>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
-      <c r="V56" s="33">
+      <c r="V56" s="29">
         <v>40</v>
       </c>
       <c r="W56" t="s">
@@ -2309,12 +2301,12 @@
       <c r="R57" t="s">
         <v>89</v>
       </c>
-      <c r="S57" s="29">
+      <c r="S57" s="25">
         <v>26</v>
       </c>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
-      <c r="V57" s="29">
+      <c r="V57" s="25">
         <v>39</v>
       </c>
       <c r="W57" t="s">
@@ -2337,12 +2329,12 @@
       <c r="R58" t="s">
         <v>90</v>
       </c>
-      <c r="S58" s="29">
+      <c r="S58" s="25">
         <v>27</v>
       </c>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
-      <c r="V58" s="29">
+      <c r="V58" s="25">
         <v>38</v>
       </c>
       <c r="W58" t="s">
@@ -2365,12 +2357,12 @@
       <c r="P59" t="s">
         <v>104</v>
       </c>
-      <c r="S59" s="29">
+      <c r="S59" s="25">
         <v>28</v>
       </c>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
-      <c r="V59" s="29">
+      <c r="V59" s="25">
         <v>37</v>
       </c>
       <c r="X59" t="s">
@@ -2390,12 +2382,12 @@
       <c r="P60" t="s">
         <v>102</v>
       </c>
-      <c r="S60" s="29">
+      <c r="S60" s="25">
         <v>29</v>
       </c>
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
-      <c r="V60" s="33">
+      <c r="V60" s="29">
         <v>36</v>
       </c>
       <c r="X60" s="4" t="s">
@@ -2415,12 +2407,12 @@
       <c r="P61" t="s">
         <v>102</v>
       </c>
-      <c r="S61" s="29">
+      <c r="S61" s="25">
         <v>30</v>
       </c>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
-      <c r="V61" s="33">
+      <c r="V61" s="29">
         <v>35</v>
       </c>
       <c r="X61" s="4" t="s">
@@ -2437,12 +2429,12 @@
       <c r="P62" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="S62" s="31">
+      <c r="S62" s="27">
         <v>31</v>
       </c>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
-      <c r="V62" s="31">
+      <c r="V62" s="27">
         <v>34</v>
       </c>
       <c r="X62" t="s">
@@ -2459,12 +2451,12 @@
       <c r="P63" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="S63" s="31">
+      <c r="S63" s="27">
         <v>32</v>
       </c>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
-      <c r="V63" s="31">
+      <c r="V63" s="27">
         <v>33</v>
       </c>
       <c r="AB63">
@@ -2536,12 +2528,12 @@
       <c r="P75" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="S75" s="31">
+      <c r="S75" s="27">
         <v>32</v>
       </c>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
-      <c r="V75" s="31">
+      <c r="V75" s="27">
         <v>33</v>
       </c>
       <c r="AB75">
@@ -2555,12 +2547,12 @@
       <c r="P76" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="S76" s="31">
+      <c r="S76" s="27">
         <v>31</v>
       </c>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
-      <c r="V76" s="31">
+      <c r="V76" s="27">
         <v>34</v>
       </c>
       <c r="X76" t="s">
@@ -2580,12 +2572,12 @@
       <c r="P77" t="s">
         <v>102</v>
       </c>
-      <c r="S77" s="29">
+      <c r="S77" s="25">
         <v>30</v>
       </c>
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
-      <c r="V77" s="33">
+      <c r="V77" s="29">
         <v>35</v>
       </c>
       <c r="X77" s="4" t="s">
@@ -2605,12 +2597,12 @@
       <c r="P78" t="s">
         <v>102</v>
       </c>
-      <c r="S78" s="29">
+      <c r="S78" s="25">
         <v>29</v>
       </c>
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
-      <c r="V78" s="33">
+      <c r="V78" s="29">
         <v>36</v>
       </c>
       <c r="X78" s="4" t="s">
@@ -2630,12 +2622,12 @@
       <c r="P79" t="s">
         <v>104</v>
       </c>
-      <c r="S79" s="29">
+      <c r="S79" s="25">
         <v>28</v>
       </c>
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
-      <c r="V79" s="29">
+      <c r="V79" s="25">
         <v>37</v>
       </c>
       <c r="X79" t="s">
@@ -2655,12 +2647,12 @@
       <c r="R80" t="s">
         <v>90</v>
       </c>
-      <c r="S80" s="29">
+      <c r="S80" s="25">
         <v>27</v>
       </c>
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
-      <c r="V80" s="29">
+      <c r="V80" s="25">
         <v>38</v>
       </c>
       <c r="W80" t="s">
@@ -2683,12 +2675,12 @@
       <c r="R81" t="s">
         <v>89</v>
       </c>
-      <c r="S81" s="29">
+      <c r="S81" s="25">
         <v>26</v>
       </c>
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
-      <c r="V81" s="29">
+      <c r="V81" s="25">
         <v>39</v>
       </c>
       <c r="W81" t="s">
@@ -2711,12 +2703,12 @@
       <c r="R82" t="s">
         <v>88</v>
       </c>
-      <c r="S82" s="29">
+      <c r="S82" s="25">
         <v>25</v>
       </c>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
-      <c r="V82" s="33">
+      <c r="V82" s="29">
         <v>40</v>
       </c>
       <c r="W82" t="s">
@@ -2733,18 +2725,18 @@
       <c r="N83">
         <v>47</v>
       </c>
-      <c r="Q83" s="37" t="s">
+      <c r="Q83" s="33" t="s">
         <v>111</v>
       </c>
       <c r="R83" t="s">
         <v>87</v>
       </c>
-      <c r="S83" s="29">
+      <c r="S83" s="25">
         <v>24</v>
       </c>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
-      <c r="V83" s="33">
+      <c r="V83" s="29">
         <v>41</v>
       </c>
       <c r="W83" t="s">
@@ -2761,12 +2753,12 @@
       <c r="N84">
         <v>48</v>
       </c>
-      <c r="S84" s="30" t="s">
+      <c r="S84" s="26" t="s">
         <v>50</v>
       </c>
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
-      <c r="V84" s="30" t="s">
+      <c r="V84" s="26" t="s">
         <v>49</v>
       </c>
       <c r="AB84">
@@ -2777,15 +2769,15 @@
       <c r="N85">
         <v>49</v>
       </c>
-      <c r="Q85" s="38" t="s">
+      <c r="Q85" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="S85" s="33">
+      <c r="S85" s="29">
         <v>12</v>
       </c>
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
-      <c r="V85" s="33">
+      <c r="V85" s="29">
         <v>13</v>
       </c>
       <c r="W85" t="s">
@@ -2802,15 +2794,15 @@
       <c r="N86">
         <v>50</v>
       </c>
-      <c r="Q86" s="38" t="s">
+      <c r="Q86" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="S86" s="33">
+      <c r="S86" s="29">
         <v>11</v>
       </c>
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
-      <c r="V86" s="29">
+      <c r="V86" s="25">
         <v>14</v>
       </c>
       <c r="W86" s="19" t="s">
@@ -2824,15 +2816,15 @@
       <c r="N87">
         <v>51</v>
       </c>
-      <c r="Q87" s="38" t="s">
+      <c r="Q87" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="S87" s="29">
+      <c r="S87" s="25">
         <v>10</v>
       </c>
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
-      <c r="V87" s="29">
+      <c r="V87" s="25">
         <v>15</v>
       </c>
       <c r="W87" s="19" t="s">
@@ -2852,12 +2844,12 @@
       <c r="P88" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="S88" s="33">
+      <c r="S88" s="29">
         <v>9</v>
       </c>
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
-      <c r="V88" s="29">
+      <c r="V88" s="25">
         <v>16</v>
       </c>
       <c r="W88" s="19" t="s">
@@ -2872,15 +2864,15 @@
       <c r="N89">
         <v>53</v>
       </c>
-      <c r="Q89" s="38" t="s">
+      <c r="Q89" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="S89" s="32">
+      <c r="S89" s="28">
         <v>8</v>
       </c>
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
-      <c r="V89" s="29">
+      <c r="V89" s="25">
         <v>17</v>
       </c>
       <c r="W89" s="19" t="s">
@@ -2894,15 +2886,15 @@
       <c r="N90">
         <v>54</v>
       </c>
-      <c r="Q90" s="38" t="s">
+      <c r="Q90" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="S90" s="32">
+      <c r="S90" s="28">
         <v>7</v>
       </c>
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
-      <c r="V90" s="29">
+      <c r="V90" s="25">
         <v>18</v>
       </c>
       <c r="W90" t="s">
@@ -2919,15 +2911,15 @@
       <c r="N91">
         <v>55</v>
       </c>
-      <c r="Q91" s="37" t="s">
+      <c r="Q91" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="S91" s="32">
+      <c r="S91" s="28">
         <v>6</v>
       </c>
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
-      <c r="V91" s="29">
+      <c r="V91" s="25">
         <v>19</v>
       </c>
       <c r="W91" t="s">
@@ -2944,12 +2936,12 @@
       <c r="N92">
         <v>56</v>
       </c>
-      <c r="S92" s="31">
+      <c r="S92" s="27">
         <v>5</v>
       </c>
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
-      <c r="V92" s="29">
+      <c r="V92" s="25">
         <v>20</v>
       </c>
       <c r="W92" t="s">
@@ -2966,12 +2958,12 @@
       <c r="N93">
         <v>57</v>
       </c>
-      <c r="S93" s="31">
+      <c r="S93" s="27">
         <v>4</v>
       </c>
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
-      <c r="V93" s="29">
+      <c r="V93" s="25">
         <v>21</v>
       </c>
       <c r="W93" t="s">
@@ -2988,12 +2980,12 @@
       <c r="N94">
         <v>58</v>
       </c>
-      <c r="S94" s="31">
+      <c r="S94" s="27">
         <v>3</v>
       </c>
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
-      <c r="V94" s="29">
+      <c r="V94" s="25">
         <v>22</v>
       </c>
       <c r="W94" s="19" t="s">
@@ -3007,12 +2999,12 @@
       <c r="N95">
         <v>59</v>
       </c>
-      <c r="S95" s="31">
+      <c r="S95" s="27">
         <v>2</v>
       </c>
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
-      <c r="V95" s="29">
+      <c r="V95" s="25">
         <v>23</v>
       </c>
       <c r="W95" t="s">
@@ -3029,12 +3021,12 @@
       <c r="N96">
         <v>60</v>
       </c>
-      <c r="S96" s="31">
+      <c r="S96" s="27">
         <v>1</v>
       </c>
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
-      <c r="V96" s="30" t="s">
+      <c r="V96" s="26" t="s">
         <v>50</v>
       </c>
       <c r="AB96">
@@ -3045,12 +3037,12 @@
       <c r="N97">
         <v>61</v>
       </c>
-      <c r="S97" s="31">
+      <c r="S97" s="27">
         <v>0</v>
       </c>
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
-      <c r="V97" s="34"/>
+      <c r="V97" s="30"/>
       <c r="W97" s="3" t="s">
         <v>49</v>
       </c>
@@ -3062,12 +3054,12 @@
       <c r="N98">
         <v>62</v>
       </c>
-      <c r="S98" s="30" t="s">
+      <c r="S98" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
-      <c r="V98" s="30" t="s">
+      <c r="V98" s="26" t="s">
         <v>52</v>
       </c>
       <c r="AB98">
@@ -3078,15 +3070,15 @@
       <c r="N102" t="s">
         <v>104</v>
       </c>
-      <c r="Q102" s="36" t="s">
+      <c r="Q102" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="S102" s="31">
+      <c r="S102" s="27">
         <v>33</v>
       </c>
       <c r="T102" s="1"/>
       <c r="U102" s="1"/>
-      <c r="V102" s="31">
+      <c r="V102" s="27">
         <v>32</v>
       </c>
       <c r="X102" s="4" t="s">
@@ -3097,15 +3089,15 @@
       <c r="N103" t="s">
         <v>103</v>
       </c>
-      <c r="Q103" s="36" t="s">
+      <c r="Q103" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="S103" s="31">
+      <c r="S103" s="27">
         <v>34</v>
       </c>
       <c r="T103" s="1"/>
       <c r="U103" s="1"/>
-      <c r="V103" s="31">
+      <c r="V103" s="27">
         <v>31</v>
       </c>
       <c r="X103" s="4" t="s">
@@ -3119,15 +3111,15 @@
       <c r="O104" t="s">
         <v>110</v>
       </c>
-      <c r="Q104" s="36" t="s">
+      <c r="Q104" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="S104" s="33">
+      <c r="S104" s="29">
         <v>35</v>
       </c>
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
-      <c r="V104" s="29">
+      <c r="V104" s="25">
         <v>30</v>
       </c>
       <c r="X104" s="4" t="s">
@@ -3141,15 +3133,15 @@
       <c r="O105" t="s">
         <v>108</v>
       </c>
-      <c r="Q105" s="36" t="s">
+      <c r="Q105" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="S105" s="33">
+      <c r="S105" s="29">
         <v>36</v>
       </c>
       <c r="T105" s="1"/>
       <c r="U105" s="1"/>
-      <c r="V105" s="29">
+      <c r="V105" s="25">
         <v>29</v>
       </c>
       <c r="X105" t="s">
@@ -3163,15 +3155,15 @@
       <c r="O106" t="s">
         <v>109</v>
       </c>
-      <c r="Q106" s="36" t="s">
+      <c r="Q106" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="S106" s="29">
+      <c r="S106" s="25">
         <v>37</v>
       </c>
       <c r="T106" s="1"/>
       <c r="U106" s="1"/>
-      <c r="V106" s="29">
+      <c r="V106" s="25">
         <v>28</v>
       </c>
       <c r="X106" t="s">
@@ -3179,18 +3171,18 @@
       </c>
     </row>
     <row r="107" spans="14:28" x14ac:dyDescent="0.3">
-      <c r="Q107" s="36" t="s">
+      <c r="Q107" s="32" t="s">
         <v>102</v>
       </c>
       <c r="R107" t="s">
         <v>91</v>
       </c>
-      <c r="S107" s="29">
+      <c r="S107" s="25">
         <v>38</v>
       </c>
       <c r="T107" s="1"/>
       <c r="U107" s="1"/>
-      <c r="V107" s="29">
+      <c r="V107" s="25">
         <v>27</v>
       </c>
       <c r="W107" t="s">
@@ -3201,18 +3193,18 @@
       </c>
     </row>
     <row r="108" spans="14:28" x14ac:dyDescent="0.3">
-      <c r="Q108" s="39" t="s">
+      <c r="Q108" s="35" t="s">
         <v>96</v>
       </c>
       <c r="R108" t="s">
         <v>92</v>
       </c>
-      <c r="S108" s="33">
+      <c r="S108" s="29">
         <v>39</v>
       </c>
       <c r="T108" s="1"/>
       <c r="U108" s="1"/>
-      <c r="V108" s="29">
+      <c r="V108" s="25">
         <v>26</v>
       </c>
       <c r="W108" t="s">
@@ -3223,18 +3215,18 @@
       </c>
     </row>
     <row r="109" spans="14:28" x14ac:dyDescent="0.3">
-      <c r="Q109" s="40" t="s">
+      <c r="Q109" s="36" t="s">
         <v>105</v>
       </c>
       <c r="R109" t="s">
         <v>94</v>
       </c>
-      <c r="S109" s="33">
+      <c r="S109" s="29">
         <v>40</v>
       </c>
       <c r="T109" s="1"/>
       <c r="U109" s="1"/>
-      <c r="V109" s="29">
+      <c r="V109" s="25">
         <v>25</v>
       </c>
       <c r="W109" t="s">
@@ -3245,18 +3237,18 @@
       </c>
     </row>
     <row r="110" spans="14:28" x14ac:dyDescent="0.3">
-      <c r="Q110" s="40" t="s">
+      <c r="Q110" s="36" t="s">
         <v>74</v>
       </c>
       <c r="R110" t="s">
         <v>93</v>
       </c>
-      <c r="S110" s="33">
+      <c r="S110" s="29">
         <v>41</v>
       </c>
       <c r="T110" s="1"/>
       <c r="U110" s="1"/>
-      <c r="V110" s="29">
+      <c r="V110" s="25">
         <v>24</v>
       </c>
       <c r="W110" t="s">
@@ -3267,28 +3259,28 @@
       </c>
     </row>
     <row r="111" spans="14:28" x14ac:dyDescent="0.3">
-      <c r="S111" s="30" t="s">
+      <c r="S111" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T111" s="1"/>
       <c r="U111" s="1"/>
-      <c r="V111" s="30" t="s">
+      <c r="V111" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="112" spans="14:28" x14ac:dyDescent="0.3">
-      <c r="Q112" s="41" t="s">
+      <c r="Q112" s="37" t="s">
         <v>31</v>
       </c>
       <c r="R112" t="s">
         <v>51</v>
       </c>
-      <c r="S112" s="33">
+      <c r="S112" s="29">
         <v>13</v>
       </c>
       <c r="T112" s="1"/>
       <c r="U112" s="1"/>
-      <c r="V112" s="33">
+      <c r="V112" s="29">
         <v>12</v>
       </c>
       <c r="X112" s="13" t="s">
@@ -3296,18 +3288,18 @@
       </c>
     </row>
     <row r="113" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="Q113" s="36" t="s">
+      <c r="Q113" s="32" t="s">
         <v>132</v>
       </c>
       <c r="R113" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="S113" s="29">
+      <c r="S113" s="25">
         <v>14</v>
       </c>
       <c r="T113" s="1"/>
       <c r="U113" s="1"/>
-      <c r="V113" s="33">
+      <c r="V113" s="29">
         <v>11</v>
       </c>
       <c r="X113" s="13" t="s">
@@ -3324,12 +3316,12 @@
       <c r="R114" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="S114" s="29">
+      <c r="S114" s="25">
         <v>15</v>
       </c>
       <c r="T114" s="1"/>
       <c r="U114" s="1"/>
-      <c r="V114" s="29">
+      <c r="V114" s="25">
         <v>10</v>
       </c>
       <c r="X114" s="13" t="s">
@@ -3340,16 +3332,16 @@
       <c r="P115" t="s">
         <v>123</v>
       </c>
-      <c r="Q115" s="42"/>
+      <c r="Q115" s="38"/>
       <c r="R115" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="S115" s="29">
+      <c r="S115" s="25">
         <v>16</v>
       </c>
       <c r="T115" s="1"/>
       <c r="U115" s="1"/>
-      <c r="V115" s="33">
+      <c r="V115" s="29">
         <v>9</v>
       </c>
       <c r="X115" t="s">
@@ -3363,12 +3355,12 @@
       <c r="R116" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="S116" s="29">
+      <c r="S116" s="25">
         <v>17</v>
       </c>
       <c r="T116" s="1"/>
       <c r="U116" s="1"/>
-      <c r="V116" s="32">
+      <c r="V116" s="28">
         <v>8</v>
       </c>
       <c r="X116" s="13" t="s">
@@ -3376,18 +3368,18 @@
       </c>
     </row>
     <row r="117" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="Q117" s="41" t="s">
+      <c r="Q117" s="37" t="s">
         <v>29</v>
       </c>
       <c r="R117" t="s">
         <v>84</v>
       </c>
-      <c r="S117" s="29">
+      <c r="S117" s="25">
         <v>18</v>
       </c>
       <c r="T117" s="1"/>
       <c r="U117" s="1"/>
-      <c r="V117" s="32">
+      <c r="V117" s="28">
         <v>7</v>
       </c>
       <c r="X117" s="13" t="s">
@@ -3395,18 +3387,18 @@
       </c>
     </row>
     <row r="118" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="Q118" s="41" t="s">
+      <c r="Q118" s="37" t="s">
         <v>26</v>
       </c>
       <c r="R118" t="s">
         <v>83</v>
       </c>
-      <c r="S118" s="29">
+      <c r="S118" s="25">
         <v>19</v>
       </c>
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
-      <c r="V118" s="32">
+      <c r="V118" s="28">
         <v>6</v>
       </c>
       <c r="X118" s="2" t="s">
@@ -3414,18 +3406,18 @@
       </c>
     </row>
     <row r="119" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="Q119" s="37" t="s">
+      <c r="Q119" s="33" t="s">
         <v>116</v>
       </c>
       <c r="R119" t="s">
         <v>82</v>
       </c>
-      <c r="S119" s="29">
+      <c r="S119" s="25">
         <v>20</v>
       </c>
       <c r="T119" s="1"/>
       <c r="U119" s="1"/>
-      <c r="V119" s="31">
+      <c r="V119" s="27">
         <v>5</v>
       </c>
       <c r="X119" t="s">
@@ -3433,18 +3425,18 @@
       </c>
     </row>
     <row r="120" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="Q120" s="37" t="s">
+      <c r="Q120" s="33" t="s">
         <v>117</v>
       </c>
       <c r="R120" t="s">
         <v>81</v>
       </c>
-      <c r="S120" s="29">
+      <c r="S120" s="25">
         <v>21</v>
       </c>
       <c r="T120" s="1"/>
       <c r="U120" s="1"/>
-      <c r="V120" s="31">
+      <c r="V120" s="27">
         <v>4</v>
       </c>
       <c r="X120" t="s">
@@ -3458,12 +3450,12 @@
       <c r="R121" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="S121" s="29">
+      <c r="S121" s="25">
         <v>22</v>
       </c>
       <c r="T121" s="1"/>
       <c r="U121" s="1"/>
-      <c r="V121" s="31">
+      <c r="V121" s="27">
         <v>3</v>
       </c>
       <c r="X121" t="s">
@@ -3471,18 +3463,18 @@
       </c>
     </row>
     <row r="122" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="Q122" s="37" t="s">
+      <c r="Q122" s="33" t="s">
         <v>118</v>
       </c>
       <c r="R122" t="s">
         <v>79</v>
       </c>
-      <c r="S122" s="29">
+      <c r="S122" s="25">
         <v>23</v>
       </c>
       <c r="T122" s="1"/>
       <c r="U122" s="1"/>
-      <c r="V122" s="31">
+      <c r="V122" s="27">
         <v>2</v>
       </c>
       <c r="X122" t="s">
@@ -3490,12 +3482,12 @@
       </c>
     </row>
     <row r="123" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="S123" s="30" t="s">
+      <c r="S123" s="26" t="s">
         <v>50</v>
       </c>
       <c r="T123" s="1"/>
       <c r="U123" s="1"/>
-      <c r="V123" s="31">
+      <c r="V123" s="27">
         <v>1</v>
       </c>
       <c r="X123" t="s">
@@ -3504,12 +3496,12 @@
     </row>
     <row r="124" spans="16:24" x14ac:dyDescent="0.3">
       <c r="R124" s="3"/>
-      <c r="S124" s="30" t="s">
+      <c r="S124" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T124" s="1"/>
       <c r="U124" s="1"/>
-      <c r="V124" s="31">
+      <c r="V124" s="27">
         <v>0</v>
       </c>
       <c r="X124" t="s">
@@ -3517,25 +3509,25 @@
       </c>
     </row>
     <row r="125" spans="16:24" x14ac:dyDescent="0.3">
-      <c r="S125" s="30" t="s">
+      <c r="S125" s="26" t="s">
         <v>52</v>
       </c>
       <c r="T125" s="1"/>
       <c r="U125" s="1"/>
-      <c r="V125" s="30" t="s">
+      <c r="V125" s="26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="129" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q129" s="40" t="s">
+      <c r="Q129" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="S129" s="33">
+      <c r="S129" s="29">
         <v>33</v>
       </c>
       <c r="T129" s="1"/>
       <c r="U129" s="1"/>
-      <c r="V129" s="29">
+      <c r="V129" s="25">
         <v>32</v>
       </c>
       <c r="X129" t="s">
@@ -3543,15 +3535,15 @@
       </c>
     </row>
     <row r="130" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q130" s="40" t="s">
+      <c r="Q130" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="S130" s="33">
+      <c r="S130" s="29">
         <v>34</v>
       </c>
       <c r="T130" s="1"/>
       <c r="U130" s="1"/>
-      <c r="V130" s="29">
+      <c r="V130" s="25">
         <v>31</v>
       </c>
       <c r="X130" t="s">
@@ -3559,15 +3551,15 @@
       </c>
     </row>
     <row r="131" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q131" s="40" t="s">
+      <c r="Q131" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="S131" s="33">
+      <c r="S131" s="29">
         <v>35</v>
       </c>
       <c r="T131" s="1"/>
       <c r="U131" s="1"/>
-      <c r="V131" s="29">
+      <c r="V131" s="25">
         <v>30</v>
       </c>
       <c r="X131" t="s">
@@ -3575,15 +3567,15 @@
       </c>
     </row>
     <row r="132" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q132" s="40" t="s">
+      <c r="Q132" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="S132" s="33">
+      <c r="S132" s="29">
         <v>36</v>
       </c>
       <c r="T132" s="1"/>
       <c r="U132" s="1"/>
-      <c r="V132" s="29">
+      <c r="V132" s="25">
         <v>29</v>
       </c>
       <c r="X132" t="s">
@@ -3591,15 +3583,15 @@
       </c>
     </row>
     <row r="133" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q133" s="40" t="s">
+      <c r="Q133" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="S133" s="33">
+      <c r="S133" s="29">
         <v>37</v>
       </c>
       <c r="T133" s="1"/>
       <c r="U133" s="1"/>
-      <c r="V133" s="29">
+      <c r="V133" s="25">
         <v>28</v>
       </c>
       <c r="X133" t="s">
@@ -3607,18 +3599,18 @@
       </c>
     </row>
     <row r="134" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q134" s="40" t="s">
+      <c r="Q134" s="36" t="s">
         <v>141</v>
       </c>
       <c r="R134" t="s">
         <v>91</v>
       </c>
-      <c r="S134" s="29">
+      <c r="S134" s="25">
         <v>38</v>
       </c>
       <c r="T134" s="1"/>
       <c r="U134" s="1"/>
-      <c r="V134" s="35">
+      <c r="V134" s="31">
         <v>27</v>
       </c>
       <c r="W134" t="s">
@@ -3629,18 +3621,18 @@
       </c>
     </row>
     <row r="135" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q135" s="39" t="s">
+      <c r="Q135" s="35" t="s">
         <v>96</v>
       </c>
       <c r="R135" t="s">
         <v>92</v>
       </c>
-      <c r="S135" s="29">
+      <c r="S135" s="25">
         <v>39</v>
       </c>
       <c r="T135" s="1"/>
       <c r="U135" s="1"/>
-      <c r="V135" s="35">
+      <c r="V135" s="31">
         <v>26</v>
       </c>
       <c r="W135" t="s">
@@ -3651,18 +3643,18 @@
       </c>
     </row>
     <row r="136" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q136" s="36" t="s">
+      <c r="Q136" s="32" t="s">
         <v>136</v>
       </c>
       <c r="R136" t="s">
         <v>94</v>
       </c>
-      <c r="S136" s="29">
+      <c r="S136" s="25">
         <v>40</v>
       </c>
       <c r="T136" s="1"/>
       <c r="U136" s="1"/>
-      <c r="V136" s="29">
+      <c r="V136" s="25">
         <v>25</v>
       </c>
       <c r="W136" t="s">
@@ -3676,18 +3668,18 @@
       <c r="O137" t="s">
         <v>142</v>
       </c>
-      <c r="Q137" s="36" t="s">
+      <c r="Q137" s="32" t="s">
         <v>135</v>
       </c>
       <c r="R137" t="s">
         <v>93</v>
       </c>
-      <c r="S137" s="29">
+      <c r="S137" s="25">
         <v>41</v>
       </c>
       <c r="T137" s="1"/>
       <c r="U137" s="1"/>
-      <c r="V137" s="29">
+      <c r="V137" s="25">
         <v>24</v>
       </c>
       <c r="W137" t="s">
@@ -3698,30 +3690,30 @@
       </c>
     </row>
     <row r="138" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q138" s="43"/>
-      <c r="S138" s="30" t="s">
+      <c r="Q138" s="39"/>
+      <c r="S138" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T138" s="1"/>
       <c r="U138" s="1"/>
-      <c r="V138" s="30" t="s">
+      <c r="V138" s="26" t="s">
         <v>50</v>
       </c>
       <c r="X138" s="22"/>
     </row>
     <row r="139" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q139" s="44" t="s">
+      <c r="Q139" s="40" t="s">
         <v>31</v>
       </c>
       <c r="R139" t="s">
         <v>51</v>
       </c>
-      <c r="S139" s="29">
+      <c r="S139" s="25">
         <v>13</v>
       </c>
       <c r="T139" s="1"/>
       <c r="U139" s="1"/>
-      <c r="V139" s="29">
+      <c r="V139" s="25">
         <v>12</v>
       </c>
       <c r="X139" s="13" t="s">
@@ -3729,18 +3721,18 @@
       </c>
     </row>
     <row r="140" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q140" s="44" t="s">
+      <c r="Q140" s="40" t="s">
         <v>132</v>
       </c>
       <c r="R140" t="s">
         <v>77</v>
       </c>
-      <c r="S140" s="29">
+      <c r="S140" s="25">
         <v>14</v>
       </c>
       <c r="T140" s="1"/>
       <c r="U140" s="1"/>
-      <c r="V140" s="29">
+      <c r="V140" s="25">
         <v>11</v>
       </c>
       <c r="X140" s="13" t="s">
@@ -3751,18 +3743,18 @@
       <c r="O141" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="Q141" s="45" t="s">
+      <c r="Q141" s="41" t="s">
         <v>123</v>
       </c>
       <c r="R141" t="s">
         <v>78</v>
       </c>
-      <c r="S141" s="29">
+      <c r="S141" s="25">
         <v>15</v>
       </c>
       <c r="T141" s="1"/>
       <c r="U141" s="1"/>
-      <c r="V141" s="29">
+      <c r="V141" s="25">
         <v>10</v>
       </c>
       <c r="X141" s="13" t="s">
@@ -3770,18 +3762,18 @@
       </c>
     </row>
     <row r="142" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q142" s="37" t="s">
+      <c r="Q142" s="33" t="s">
         <v>111</v>
       </c>
       <c r="R142" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="S142" s="29">
+      <c r="S142" s="25">
         <v>16</v>
       </c>
       <c r="T142" s="1"/>
       <c r="U142" s="1"/>
-      <c r="V142" s="29">
+      <c r="V142" s="25">
         <v>9</v>
       </c>
       <c r="X142" t="s">
@@ -3789,18 +3781,18 @@
       </c>
     </row>
     <row r="143" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q143" s="45" t="s">
+      <c r="Q143" s="41" t="s">
         <v>124</v>
       </c>
       <c r="R143" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="S143" s="29">
+      <c r="S143" s="25">
         <v>17</v>
       </c>
       <c r="T143" s="1"/>
       <c r="U143" s="1"/>
-      <c r="V143" s="32">
+      <c r="V143" s="28">
         <v>8</v>
       </c>
       <c r="X143" s="13" t="s">
@@ -3808,18 +3800,18 @@
       </c>
     </row>
     <row r="144" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="Q144" s="41" t="s">
+      <c r="Q144" s="37" t="s">
         <v>29</v>
       </c>
       <c r="R144" t="s">
         <v>84</v>
       </c>
-      <c r="S144" s="29">
+      <c r="S144" s="25">
         <v>18</v>
       </c>
       <c r="T144" s="1"/>
       <c r="U144" s="1"/>
-      <c r="V144" s="32">
+      <c r="V144" s="28">
         <v>7</v>
       </c>
       <c r="X144" s="13" t="s">
@@ -3827,18 +3819,18 @@
       </c>
     </row>
     <row r="145" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="Q145" s="41" t="s">
+      <c r="Q145" s="37" t="s">
         <v>26</v>
       </c>
       <c r="R145" t="s">
         <v>83</v>
       </c>
-      <c r="S145" s="29">
+      <c r="S145" s="25">
         <v>19</v>
       </c>
       <c r="T145" s="1"/>
       <c r="U145" s="1"/>
-      <c r="V145" s="32">
+      <c r="V145" s="28">
         <v>6</v>
       </c>
       <c r="X145" s="2" t="s">
@@ -3846,18 +3838,18 @@
       </c>
     </row>
     <row r="146" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="Q146" s="37" t="s">
+      <c r="Q146" s="33" t="s">
         <v>116</v>
       </c>
       <c r="R146" t="s">
         <v>82</v>
       </c>
-      <c r="S146" s="29">
+      <c r="S146" s="25">
         <v>20</v>
       </c>
       <c r="T146" s="1"/>
       <c r="U146" s="1"/>
-      <c r="V146" s="29">
+      <c r="V146" s="25">
         <v>5</v>
       </c>
       <c r="X146" t="s">
@@ -3865,18 +3857,18 @@
       </c>
     </row>
     <row r="147" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="Q147" s="37" t="s">
+      <c r="Q147" s="33" t="s">
         <v>117</v>
       </c>
       <c r="R147" t="s">
         <v>81</v>
       </c>
-      <c r="S147" s="29">
+      <c r="S147" s="25">
         <v>21</v>
       </c>
       <c r="T147" s="1"/>
       <c r="U147" s="1"/>
-      <c r="V147" s="29">
+      <c r="V147" s="25">
         <v>4</v>
       </c>
       <c r="X147" t="s">
@@ -3884,18 +3876,18 @@
       </c>
     </row>
     <row r="148" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="Q148" s="44" t="s">
+      <c r="Q148" s="40" t="s">
         <v>139</v>
       </c>
       <c r="R148" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="S148" s="29">
+      <c r="S148" s="25">
         <v>22</v>
       </c>
       <c r="T148" s="1"/>
       <c r="U148" s="1"/>
-      <c r="V148" s="29">
+      <c r="V148" s="25">
         <v>3</v>
       </c>
       <c r="X148" t="s">
@@ -3903,18 +3895,18 @@
       </c>
     </row>
     <row r="149" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="Q149" s="37" t="s">
+      <c r="Q149" s="33" t="s">
         <v>118</v>
       </c>
       <c r="R149" t="s">
         <v>79</v>
       </c>
-      <c r="S149" s="29">
+      <c r="S149" s="25">
         <v>23</v>
       </c>
       <c r="T149" s="1"/>
       <c r="U149" s="1"/>
-      <c r="V149" s="29">
+      <c r="V149" s="25">
         <v>2</v>
       </c>
       <c r="X149" s="24" t="s">
@@ -3922,12 +3914,12 @@
       </c>
     </row>
     <row r="150" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="S150" s="30" t="s">
+      <c r="S150" s="26" t="s">
         <v>50</v>
       </c>
       <c r="T150" s="1"/>
       <c r="U150" s="1"/>
-      <c r="V150" s="35">
+      <c r="V150" s="31">
         <v>1</v>
       </c>
       <c r="X150" t="s">
@@ -3936,12 +3928,12 @@
     </row>
     <row r="151" spans="14:24" x14ac:dyDescent="0.3">
       <c r="R151" s="3"/>
-      <c r="S151" s="30" t="s">
+      <c r="S151" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T151" s="1"/>
       <c r="U151" s="1"/>
-      <c r="V151" s="29">
+      <c r="V151" s="25">
         <v>0</v>
       </c>
       <c r="X151" t="s">
@@ -3949,197 +3941,197 @@
       </c>
     </row>
     <row r="152" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="S152" s="30" t="s">
+      <c r="S152" s="26" t="s">
         <v>52</v>
       </c>
       <c r="T152" s="1"/>
       <c r="U152" s="1"/>
-      <c r="V152" s="30" t="s">
+      <c r="V152" s="26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="155" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="N155" s="40"/>
+      <c r="N155" s="36"/>
       <c r="O155" t="s">
         <v>154</v>
       </c>
-      <c r="Q155" s="40" t="s">
+      <c r="Q155" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="S155" s="33">
+      <c r="S155" s="29">
         <v>33</v>
       </c>
       <c r="T155" s="1"/>
       <c r="U155" s="1"/>
-      <c r="V155" s="31">
+      <c r="V155" s="27">
         <v>32</v>
       </c>
-      <c r="X155" s="58" t="s">
+      <c r="X155" s="52" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="156" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="N156" s="41"/>
+      <c r="N156" s="37"/>
       <c r="O156" t="s">
         <v>155</v>
       </c>
-      <c r="Q156" s="40" t="s">
+      <c r="Q156" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="S156" s="33">
+      <c r="S156" s="29">
         <v>34</v>
       </c>
       <c r="T156" s="1"/>
       <c r="U156" s="1"/>
-      <c r="V156" s="31">
+      <c r="V156" s="27">
         <v>31</v>
       </c>
-      <c r="X156" s="58" t="s">
+      <c r="X156" s="52" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="157" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="N157" s="44"/>
+      <c r="N157" s="40"/>
       <c r="O157" t="s">
         <v>156</v>
       </c>
-      <c r="Q157" s="40" t="s">
+      <c r="Q157" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="S157" s="33">
+      <c r="S157" s="29">
         <v>35</v>
       </c>
       <c r="T157" s="1"/>
       <c r="U157" s="1"/>
-      <c r="V157" s="31">
+      <c r="V157" s="27">
         <v>30</v>
       </c>
-      <c r="X157" s="58" t="s">
+      <c r="X157" s="52" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="158" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="N158" s="51"/>
+      <c r="N158" s="47"/>
       <c r="O158" t="s">
         <v>157</v>
       </c>
-      <c r="Q158" s="40" t="s">
+      <c r="Q158" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="S158" s="33">
+      <c r="S158" s="29">
         <v>36</v>
       </c>
       <c r="T158" s="1"/>
       <c r="U158" s="1"/>
-      <c r="V158" s="31">
+      <c r="V158" s="27">
         <v>29</v>
       </c>
-      <c r="X158" s="58" t="s">
+      <c r="X158" s="52" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="159" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="N159" s="45"/>
+      <c r="N159" s="41"/>
       <c r="O159" t="s">
         <v>160</v>
       </c>
-      <c r="Q159" s="40" t="s">
+      <c r="Q159" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="S159" s="33">
+      <c r="S159" s="29">
         <v>37</v>
       </c>
       <c r="T159" s="1"/>
       <c r="U159" s="1"/>
-      <c r="V159" s="31">
+      <c r="V159" s="27">
         <v>28</v>
       </c>
-      <c r="X159" s="58" t="s">
+      <c r="X159" s="52" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="160" spans="14:24" x14ac:dyDescent="0.3">
-      <c r="Q160" s="40" t="s">
+      <c r="Q160" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="R160" s="55" t="s">
+      <c r="R160" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="S160" s="33">
+      <c r="S160" s="29">
         <v>38</v>
       </c>
       <c r="T160" s="1"/>
       <c r="U160" s="1"/>
-      <c r="V160" s="59">
+      <c r="V160" s="29">
         <v>27</v>
       </c>
-      <c r="W160" s="55" t="s">
+      <c r="W160" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="X160" s="54" t="s">
+      <c r="X160" s="4" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="161" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q161" s="53" t="s">
+      <c r="Q161" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="R161" s="55" t="s">
+      <c r="R161" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="S161" s="33">
+      <c r="S161" s="29">
         <v>39</v>
       </c>
       <c r="T161" s="1"/>
       <c r="U161" s="1"/>
-      <c r="V161" s="59">
+      <c r="V161" s="29">
         <v>26</v>
       </c>
-      <c r="W161" s="55" t="s">
+      <c r="W161" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="X161" s="54" t="s">
+      <c r="X161" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="162" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q162" s="52" t="s">
+      <c r="Q162" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="R162" s="55" t="s">
+      <c r="R162" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="S162" s="34">
+      <c r="S162" s="30">
         <v>40</v>
       </c>
       <c r="T162" s="1"/>
       <c r="U162" s="1"/>
-      <c r="V162" s="31">
+      <c r="V162" s="27">
         <v>25</v>
       </c>
-      <c r="W162" s="55" t="s">
+      <c r="W162" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="X162" s="58" t="s">
+      <c r="X162" s="52" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="163" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q163" s="52" t="s">
+      <c r="Q163" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="R163" s="55" t="s">
+      <c r="R163" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="S163" s="34">
+      <c r="S163" s="30">
         <v>41</v>
       </c>
       <c r="T163" s="1"/>
       <c r="U163" s="1"/>
-      <c r="V163" s="34">
+      <c r="V163" s="30">
         <v>24</v>
       </c>
-      <c r="W163" s="55" t="s">
+      <c r="W163" s="49" t="s">
         <v>87</v>
       </c>
       <c r="X163" s="1" t="s">
@@ -4147,31 +4139,31 @@
       </c>
     </row>
     <row r="164" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q164" s="43"/>
-      <c r="R164" s="55"/>
-      <c r="S164" s="30" t="s">
+      <c r="Q164" s="39"/>
+      <c r="R164" s="49"/>
+      <c r="S164" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T164" s="1"/>
       <c r="U164" s="1"/>
-      <c r="V164" s="30" t="s">
+      <c r="V164" s="26" t="s">
         <v>50</v>
       </c>
       <c r="X164" s="22"/>
     </row>
     <row r="165" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q165" s="44" t="s">
+      <c r="Q165" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="R165" s="55" t="s">
+      <c r="R165" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="S165" s="29">
+      <c r="S165" s="25">
         <v>13</v>
       </c>
       <c r="T165" s="1"/>
       <c r="U165" s="1"/>
-      <c r="V165" s="29">
+      <c r="V165" s="25">
         <v>12</v>
       </c>
       <c r="X165" s="13" t="s">
@@ -4179,18 +4171,18 @@
       </c>
     </row>
     <row r="166" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q166" s="44" t="s">
+      <c r="Q166" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="R166" s="55" t="s">
+      <c r="R166" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="S166" s="29">
+      <c r="S166" s="25">
         <v>14</v>
       </c>
       <c r="T166" s="1"/>
       <c r="U166" s="1"/>
-      <c r="V166" s="29">
+      <c r="V166" s="25">
         <v>11</v>
       </c>
       <c r="X166" s="13" t="s">
@@ -4198,18 +4190,18 @@
       </c>
     </row>
     <row r="167" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q167" s="45" t="s">
+      <c r="Q167" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="R167" s="55" t="s">
+      <c r="R167" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="S167" s="31">
+      <c r="S167" s="27">
         <v>15</v>
       </c>
       <c r="T167" s="1"/>
       <c r="U167" s="1"/>
-      <c r="V167" s="29">
+      <c r="V167" s="25">
         <v>10</v>
       </c>
       <c r="X167" s="13" t="s">
@@ -4217,18 +4209,18 @@
       </c>
     </row>
     <row r="168" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q168" s="45" t="s">
+      <c r="Q168" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="R168" s="55" t="s">
+      <c r="R168" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="S168" s="31">
+      <c r="S168" s="27">
         <v>16</v>
       </c>
       <c r="T168" s="1"/>
       <c r="U168" s="1"/>
-      <c r="V168" s="34">
+      <c r="V168" s="30">
         <v>9</v>
       </c>
       <c r="X168" s="1" t="s">
@@ -4236,18 +4228,18 @@
       </c>
     </row>
     <row r="169" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q169" s="45" t="s">
+      <c r="Q169" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="R169" s="55" t="s">
+      <c r="R169" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="S169" s="31">
+      <c r="S169" s="27">
         <v>17</v>
       </c>
       <c r="T169" s="1"/>
       <c r="U169" s="1"/>
-      <c r="V169" s="29">
+      <c r="V169" s="25">
         <v>8</v>
       </c>
       <c r="X169" s="13" t="s">
@@ -4255,18 +4247,18 @@
       </c>
     </row>
     <row r="170" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q170" s="41" t="s">
+      <c r="Q170" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="R170" s="55" t="s">
+      <c r="R170" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="S170" s="29">
+      <c r="S170" s="25">
         <v>18</v>
       </c>
       <c r="T170" s="1"/>
       <c r="U170" s="1"/>
-      <c r="V170" s="29">
+      <c r="V170" s="25">
         <v>7</v>
       </c>
       <c r="X170" s="13" t="s">
@@ -4274,18 +4266,18 @@
       </c>
     </row>
     <row r="171" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q171" s="41" t="s">
+      <c r="Q171" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="R171" s="55" t="s">
+      <c r="R171" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="S171" s="29">
+      <c r="S171" s="25">
         <v>19</v>
       </c>
       <c r="T171" s="1"/>
       <c r="U171" s="1"/>
-      <c r="V171" s="29">
+      <c r="V171" s="25">
         <v>6</v>
       </c>
       <c r="X171" s="13" t="s">
@@ -4293,75 +4285,75 @@
       </c>
     </row>
     <row r="172" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q172" s="56" t="s">
+      <c r="Q172" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="R172" s="55" t="s">
+      <c r="R172" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="S172" s="29">
+      <c r="S172" s="25">
         <v>20</v>
       </c>
       <c r="T172" s="1"/>
       <c r="U172" s="1"/>
-      <c r="V172" s="29">
+      <c r="V172" s="25">
         <v>5</v>
       </c>
-      <c r="X172" s="46" t="s">
+      <c r="X172" s="42" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="173" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q173" s="56" t="s">
+      <c r="Q173" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="R173" s="55" t="s">
+      <c r="R173" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="S173" s="29">
+      <c r="S173" s="25">
         <v>21</v>
       </c>
       <c r="T173" s="1"/>
       <c r="U173" s="1"/>
-      <c r="V173" s="29">
+      <c r="V173" s="25">
         <v>4</v>
       </c>
-      <c r="X173" s="46" t="s">
+      <c r="X173" s="42" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="174" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q174" s="44" t="s">
+      <c r="Q174" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="R174" s="55" t="s">
+      <c r="R174" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="S174" s="57">
+      <c r="S174" s="51">
         <v>22</v>
       </c>
       <c r="T174" s="1"/>
       <c r="U174" s="1"/>
-      <c r="V174" s="29">
+      <c r="V174" s="25">
         <v>3</v>
       </c>
-      <c r="X174" s="46" t="s">
+      <c r="X174" s="42" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="175" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="Q175" s="56" t="s">
+      <c r="Q175" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="R175" s="55" t="s">
+      <c r="R175" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="S175" s="29">
+      <c r="S175" s="25">
         <v>23</v>
       </c>
       <c r="T175" s="1"/>
       <c r="U175" s="1"/>
-      <c r="V175" s="57">
+      <c r="V175" s="51">
         <v>2</v>
       </c>
       <c r="X175" s="24" t="s">
@@ -4369,39 +4361,39 @@
       </c>
     </row>
     <row r="176" spans="17:24" x14ac:dyDescent="0.3">
-      <c r="S176" s="30" t="s">
+      <c r="S176" s="26" t="s">
         <v>50</v>
       </c>
       <c r="T176" s="1"/>
       <c r="U176" s="1"/>
-      <c r="V176" s="59">
+      <c r="V176" s="29">
         <v>1</v>
       </c>
-      <c r="X176" s="60" t="s">
+      <c r="X176" s="4" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="177" spans="18:24" x14ac:dyDescent="0.3">
       <c r="R177" s="3"/>
-      <c r="S177" s="30" t="s">
+      <c r="S177" s="26" t="s">
         <v>49</v>
       </c>
       <c r="T177" s="1"/>
       <c r="U177" s="1"/>
-      <c r="V177" s="31">
+      <c r="V177" s="27">
         <v>0</v>
       </c>
-      <c r="X177" s="58" t="s">
+      <c r="X177" s="52" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="178" spans="18:24" x14ac:dyDescent="0.3">
-      <c r="S178" s="30" t="s">
+      <c r="S178" s="26" t="s">
         <v>52</v>
       </c>
       <c r="T178" s="1"/>
       <c r="U178" s="1"/>
-      <c r="V178" s="30" t="s">
+      <c r="V178" s="26" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4410,6 +4402,26 @@
     <sortCondition ref="N75:N98"/>
   </sortState>
   <mergeCells count="35">
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="K26:K27"/>
     <mergeCell ref="G20:G21"/>
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="J10:J11"/>
@@ -4425,26 +4437,6 @@
     <mergeCell ref="K16:K17"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="J18:J19"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="K30:K31"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>